<commit_message>
added functionality to write performance report in excel file
</commit_message>
<xml_diff>
--- a/OutputFiles/PerformanceReport.xlsx
+++ b/OutputFiles/PerformanceReport.xlsx
@@ -2,28 +2,41 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="abc" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="PerformanceReport" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Logs" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -37,12 +50,42 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -55,14 +98,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -425,7 +474,66 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="n"/>
+      <c r="C1" s="1" t="n"/>
+      <c r="D1" s="1" t="n"/>
+      <c r="E1" s="1" t="n"/>
+      <c r="F1" s="1" t="n"/>
+      <c r="G1" s="1" t="n"/>
+      <c r="H1" s="1" t="n"/>
+      <c r="I1" s="1" t="n"/>
+      <c r="J1" s="1" t="n"/>
+      <c r="K1" s="1" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>sdfdsf</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>sdfds</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>sd</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,161 +542,155 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1" t="n">
+      <c r="A1" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G1" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H1" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I1" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J1" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Work</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>PhysicalActivities</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>PhysicalActivities</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Relationships</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>PhysicalActivities</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Learning</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Youtube</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Relationships</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>PhysicalActivities</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>PhysicalActivities</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Relationships</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>PhysicalActivities</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Learning</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Youtube</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Relationships</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Work</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ApplicationsSubmitted</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>HoursOfSalsa</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>HoursFighting</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>HoursSpentTalkingToFamily</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>HoursTraining</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>HoursSpentReading</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>MinutesOfUploadedContent</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>ad-hoc</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>HoursFighting</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>HoursOfSalsa</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>HoursSpentTalkingToFamily</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>HoursTraining</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>HoursSpentReading</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>MinutesOfUploadedContent</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>ad-hoc</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>ApplicationsSubmitted</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-    </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>Sunday, 4 September 2022</t>
         </is>
       </c>
+      <c r="B4" t="n">
+        <v>10</v>
+      </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>18.33333333333333</v>
       </c>
       <c r="D4" t="n">
-        <v>18.33333333333333</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>0.2222222222222222</v>
@@ -606,9 +708,195 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
+        <v>54.55555555555556</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G1" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H1" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I1" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J1" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Work</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>PhysicalActivities</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Relationships</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>PhysicalActivities</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>PhysicalActivities</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Learning</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Youtube</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Relationships</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ApplicationsSubmitted</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>HoursFighting</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>HoursSpentTalkingToFamily</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>HoursTraining</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>HoursOfSalsa</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>HoursSpentReading</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>MinutesOfUploadedContent</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>ad-hoc</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Sunday, 4 September 2022</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>10</v>
       </c>
-      <c r="K4" t="n">
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="E4" t="n">
+        <v>6</v>
+      </c>
+      <c r="F4" t="n">
+        <v>18.33333333333333</v>
+      </c>
+      <c r="G4" t="n">
+        <v>20</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
         <v>54.55555555555556</v>
       </c>
     </row>

</xml_diff>